<commit_message>
Minor changes to test files
</commit_message>
<xml_diff>
--- a/tests/Test_bank_statement.xlsx
+++ b/tests/Test_bank_statement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofie\Dropbox\Finance\Financial_Overview\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofie\Dropbox\Finance\Financial_Overview\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAFB075F-5944-45E4-8C53-BDBAC2678877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A138AD0-C92E-498E-89F7-BF297D9C04FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{467B606C-66AA-4C84-8CDA-8E8C7B770CD4}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{467B606C-66AA-4C84-8CDA-8E8C7B770CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t xml:space="preserve">XXXX XXXX XXXX XXXX: </t>
   </si>
   <si>
-    <t>01/01/2024 to 31/01/2024</t>
-  </si>
-  <si>
     <t>CARD PAYMENT TO TESCO ON 01-01-2024</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>DIRECT DEBIT PAYMENT TO Phone Company</t>
+  </si>
+  <si>
+    <t>01/01/2024 to 31/02/2025</t>
   </si>
 </sst>
 </file>
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -167,16 +167,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,7 +513,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -543,7 +542,7 @@
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -598,7 +597,7 @@
       </c>
       <c r="C7" s="11"/>
       <c r="D7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="5"/>
@@ -618,7 +617,7 @@
       </c>
       <c r="C8" s="11"/>
       <c r="D8" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="6">
@@ -636,8 +635,8 @@
       <c r="B9" s="12">
         <v>45296</v>
       </c>
-      <c r="D9" s="13" t="s">
-        <v>10</v>
+      <c r="D9" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="G9" s="6">
         <v>40</v>
@@ -651,8 +650,8 @@
       <c r="B10" s="12">
         <v>45296</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>11</v>
+      <c r="D10" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="G10" s="6">
         <v>100</v>
@@ -667,7 +666,7 @@
         <v>45322</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="6">
         <v>10</v>

</xml_diff>

<commit_message>
Updated test files for more functionalities
</commit_message>
<xml_diff>
--- a/tests/Test_bank_statement.xlsx
+++ b/tests/Test_bank_statement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofie\Dropbox\Finance\Financial_Overview\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A138AD0-C92E-498E-89F7-BF297D9C04FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E40292-19B1-4628-BADD-F8BF7B4E0EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{467B606C-66AA-4C84-8CDA-8E8C7B770CD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{467B606C-66AA-4C84-8CDA-8E8C7B770CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Transactions</t>
   </si>
@@ -74,7 +74,13 @@
     <t>DIRECT DEBIT PAYMENT TO Phone Company</t>
   </si>
   <si>
-    <t>01/01/2024 to 31/02/2025</t>
+    <t>01/01/2024 to 31/01/2025</t>
+  </si>
+  <si>
+    <t>CARD PAYMENT TO Netflix ON 05-01-2024</t>
+  </si>
+  <si>
+    <t>DIRECT DEBIT PAYMENT TO Rent</t>
   </si>
 </sst>
 </file>
@@ -510,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF416BC-A618-47B0-BBE9-2A1055AAE534}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -663,10 +669,10 @@
     </row>
     <row r="11" spans="1:10">
       <c r="B11" s="12">
-        <v>45322</v>
+        <v>45296</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G11" s="6">
         <v>10</v>
@@ -674,6 +680,36 @@
       <c r="H11" s="6">
         <f>SUM(H10,F11,-G11)</f>
         <v>950</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="B12" s="12">
+        <v>45322</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="6">
+        <v>10</v>
+      </c>
+      <c r="H12" s="6">
+        <f>SUM(H10,F12,-G12)</f>
+        <v>950</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="B13" s="12">
+        <v>45322</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="6">
+        <v>450</v>
+      </c>
+      <c r="H13" s="6">
+        <f>SUM(H11,F13,-G13)</f>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified test documents for more complexity in tests
</commit_message>
<xml_diff>
--- a/tests/Test_bank_statement.xlsx
+++ b/tests/Test_bank_statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sofie\Dropbox\Finance\Financial_Overview\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E40292-19B1-4628-BADD-F8BF7B4E0EE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ECF6A6B-50A5-4376-B354-049D8D90A98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{467B606C-66AA-4C84-8CDA-8E8C7B770CD4}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{467B606C-66AA-4C84-8CDA-8E8C7B770CD4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Transactions</t>
   </si>
@@ -74,21 +74,25 @@
     <t>DIRECT DEBIT PAYMENT TO Phone Company</t>
   </si>
   <si>
-    <t>01/01/2024 to 31/01/2025</t>
-  </si>
-  <si>
     <t>CARD PAYMENT TO Netflix ON 05-01-2024</t>
   </si>
   <si>
     <t>DIRECT DEBIT PAYMENT TO Rent</t>
+  </si>
+  <si>
+    <t>01/01/2024 to 31/01/2024</t>
+  </si>
+  <si>
+    <t>CREDIT FROM work</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -150,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -182,6 +186,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF416BC-A618-47B0-BBE9-2A1055AAE534}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -548,7 +553,7 @@
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
@@ -672,7 +677,7 @@
         <v>45296</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="6">
         <v>10</v>
@@ -684,35 +689,49 @@
     </row>
     <row r="12" spans="1:10">
       <c r="B12" s="12">
-        <v>45322</v>
+        <v>45306</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="6">
-        <v>10</v>
-      </c>
-      <c r="H12" s="6">
-        <f>SUM(H10,F12,-G12)</f>
-        <v>950</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="F12" s="13">
+        <v>1000</v>
+      </c>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:10">
       <c r="B13" s="12">
         <v>45322</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G13" s="6">
+        <v>10</v>
+      </c>
+      <c r="H13" s="6">
+        <f>SUM(H10,F13,-G13)</f>
+        <v>950</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="12">
+        <v>45322</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="6">
         <v>450</v>
       </c>
-      <c r="H13" s="6">
-        <f>SUM(H11,F13,-G13)</f>
+      <c r="H14" s="6">
+        <f>SUM(H11,F14,-G14)</f>
         <v>500</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>